<commit_message>
JAN 1 Presenti Sheet
JAN 1 Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -453,7 +453,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,9 @@
       <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -560,7 +562,9 @@
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -588,7 +592,9 @@
       <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -616,7 +622,9 @@
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>

</xml_diff>

<commit_message>
2 Jan Presenti sheet
2 Jan Presenti sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -54,10 +54,10 @@
     <t>Dipti Shelavane</t>
   </si>
   <si>
-    <t>Note: Time 5 PM to 7 PM</t>
-  </si>
-  <si>
     <t>Absent</t>
+  </si>
+  <si>
+    <t>Time : 5PM To 7 PM</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,9 @@
       <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -560,12 +562,14 @@
         <v>6</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7"/>
+      <c r="E3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
@@ -590,12 +594,14 @@
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -625,7 +631,9 @@
       <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -644,7 +652,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 Jan Presenti Sheet
3 Jan Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -24,8 +24,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>A</author>
+  </authors>
+  <commentList>
+    <comment ref="F5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+College Event</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -64,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,6 +112,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -449,11 +496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -538,7 +585,9 @@
       <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -570,7 +619,9 @@
       <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -602,7 +653,9 @@
       <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
@@ -634,7 +687,9 @@
       <c r="E5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -657,11 +712,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F5">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
4 Jan Presenti Sheet
4 Jan Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -30,6 +30,30 @@
     <author>A</author>
   </authors>
   <commentList>
+    <comment ref="G2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
@@ -59,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -500,7 +524,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -588,7 +612,9 @@
       <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -622,7 +648,9 @@
       <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
@@ -656,7 +684,9 @@
       <c r="F4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -690,7 +720,9 @@
       <c r="F5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
@@ -712,7 +744,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:F5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:G5">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
17 Jan presenti sheet
17 Jan presenti sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -54,6 +54,174 @@
         </r>
       </text>
     </comment>
+    <comment ref="H2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>A:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+university Exam</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
@@ -83,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -523,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -590,8 +758,12 @@
       <c r="R1" s="4">
         <v>45306</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
+      <c r="S1" s="4">
+        <v>45307</v>
+      </c>
+      <c r="T1" s="4">
+        <v>45308</v>
+      </c>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
@@ -615,19 +787,45 @@
       <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="H2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
@@ -651,19 +849,45 @@
       <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
+      <c r="H3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
@@ -687,19 +911,45 @@
       <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
+      <c r="H4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
@@ -723,19 +973,45 @@
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
@@ -744,7 +1020,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:G5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:T5">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
18 jan presenti sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -764,8 +764,11 @@
       <c r="T1" s="4">
         <v>45308</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="U1" s="4">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -826,8 +829,11 @@
       <c r="T2" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="U2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -888,8 +894,11 @@
       <c r="T3" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="U3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -950,8 +959,11 @@
       <c r="T4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="U4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1012,15 +1024,18 @@
       <c r="T5" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U5" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:T5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:U5">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
19 jan presenti sheet
19 jan presenti sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O15" activeCellId="1" sqref="P8 O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -767,8 +767,11 @@
       <c r="U1" s="4">
         <v>45309</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V1" s="4">
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -832,8 +835,11 @@
       <c r="U2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -897,8 +903,11 @@
       <c r="U3" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V3" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -962,8 +971,11 @@
       <c r="U4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="V4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1009,33 +1021,15 @@
       <c r="O5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:U5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:V4 C5:P5">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
20,21,22 jan Presenti sheet
20,21,22 jan Presenti sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O15" activeCellId="1" sqref="P8 O15"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -770,8 +770,17 @@
       <c r="V1" s="4">
         <v>45310</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W1" s="4">
+        <v>45311</v>
+      </c>
+      <c r="X1" s="4">
+        <v>45312</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>45313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -838,8 +847,17 @@
       <c r="V2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -906,8 +924,17 @@
       <c r="V3" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -974,8 +1001,17 @@
       <c r="V4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="W4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1022,14 +1058,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:V4 C5:P5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:Y4">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
24 Jan presenti sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -779,8 +779,14 @@
       <c r="Y1" s="4">
         <v>45313</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Z1" s="4">
+        <v>45314</v>
+      </c>
+      <c r="AA1" s="4">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -856,8 +862,14 @@
       <c r="Y2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Z2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -933,8 +945,14 @@
       <c r="Y3" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Z3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1010,8 +1028,14 @@
       <c r="Y4" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Z4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1058,14 +1082,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:Y4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:AA4">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
29 Jan Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB8" sqref="AB8"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -791,8 +791,17 @@
       <c r="AC1" s="4">
         <v>45317</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD1" s="4">
+        <v>45318</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>45319</v>
+      </c>
+      <c r="AF1" s="4">
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -880,8 +889,17 @@
       <c r="AC2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -969,8 +987,17 @@
       <c r="AC3" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1058,8 +1085,17 @@
       <c r="AC4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AD4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1106,14 +1142,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:AC4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:AF4">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
30 Jan Presenti Sheet
30 Jan Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AG9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH7" sqref="AH7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -800,8 +800,11 @@
       <c r="AF1" s="4">
         <v>45320</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AG1" s="4">
+        <v>45321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -898,8 +901,11 @@
       <c r="AF2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AG2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -996,8 +1002,11 @@
       <c r="AF3" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AG3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1094,8 +1103,11 @@
       <c r="AF4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AG4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1142,14 +1154,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:AF4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:AG4">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
31 Jan Presenti Sheet
31 Jan Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -689,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH7" sqref="AH7"/>
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
     <col min="8" max="8" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -803,8 +803,11 @@
       <c r="AG1" s="4">
         <v>45321</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AH1" s="4">
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -904,8 +907,11 @@
       <c r="AG2" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AH2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1005,8 +1011,11 @@
       <c r="AG3" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AH3" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1106,8 +1115,11 @@
       <c r="AG4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AH4" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1154,14 +1166,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:AG4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:P5 C2:AH4">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
1 February Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jan-2024" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="9">
   <si>
     <t>Student Name</t>
   </si>
@@ -259,13 +259,7 @@
     <t>Sr. No</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>Present</t>
-  </si>
-  <si>
-    <t>Reason</t>
   </si>
   <si>
     <t>Pratiksha Bhuse(TL)</t>
@@ -360,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,7 +364,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -691,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -808,367 +801,367 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH2" s="7" t="s">
-        <v>3</v>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="W3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="X3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH3" s="7" t="s">
-        <v>3</v>
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AG4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AH4" s="7" t="s">
-        <v>9</v>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>9</v>
+      <c r="B5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1184,15 +1177,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1200,106 +1193,174 @@
         <v>0</v>
       </c>
       <c r="C1" s="4">
-        <v>45289</v>
-      </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+        <v>45323</v>
+      </c>
+      <c r="D1" s="4">
+        <v>45324</v>
+      </c>
+      <c r="E1" s="4">
+        <v>45325</v>
+      </c>
+      <c r="F1" s="4">
+        <v>45326</v>
+      </c>
+      <c r="G1" s="4">
+        <v>45327</v>
+      </c>
+      <c r="H1" s="4">
+        <v>45328</v>
+      </c>
+      <c r="I1" s="4">
+        <v>45329</v>
+      </c>
+      <c r="J1" s="4">
+        <v>45330</v>
+      </c>
+      <c r="K1" s="4">
+        <v>45331</v>
+      </c>
+      <c r="L1" s="4">
+        <v>45332</v>
+      </c>
+      <c r="M1" s="4">
+        <v>45333</v>
+      </c>
+      <c r="N1" s="4">
+        <v>45334</v>
+      </c>
+      <c r="O1" s="4">
+        <v>45335</v>
+      </c>
+      <c r="P1" s="4">
+        <v>45336</v>
+      </c>
+      <c r="Q1" s="4">
+        <v>45337</v>
+      </c>
+      <c r="R1" s="4">
+        <v>45338</v>
+      </c>
+      <c r="S1" s="4">
+        <v>45339</v>
+      </c>
+      <c r="T1" s="4">
+        <v>45340</v>
+      </c>
+      <c r="U1" s="4">
+        <v>45341</v>
+      </c>
+      <c r="V1" s="4">
+        <v>45342</v>
+      </c>
+      <c r="W1" s="4">
+        <v>45343</v>
+      </c>
+      <c r="X1" s="4">
+        <v>45344</v>
+      </c>
+      <c r="Y1" s="4">
+        <v>45345</v>
+      </c>
+      <c r="Z1" s="4">
+        <v>45346</v>
+      </c>
+      <c r="AA1" s="4">
+        <v>45347</v>
+      </c>
+      <c r="AB1" s="4">
+        <v>45348</v>
+      </c>
+      <c r="AC1" s="4">
+        <v>45349</v>
+      </c>
+      <c r="AD1" s="4">
+        <v>45350</v>
+      </c>
+      <c r="AE1" s="4">
+        <v>45351</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+    <row r="2" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+    </row>
+    <row r="3" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9 E2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:AE2 C2:C3 F3:AE3">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
2 February Presenti Sheet
2 February Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="9">
   <si>
     <t>Student Name</t>
   </si>
@@ -1180,7 +1180,7 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1290,9 @@
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1329,7 +1331,9 @@
       <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1360,7 +1364,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:AE2 C2:C3 F3:AE3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:AE2 C2:C3 F3:AE3 D3">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
3 february Presenti Sheet
3 february Presenti Sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="9">
   <si>
     <t>Student Name</t>
   </si>
@@ -383,6 +383,81 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>829235</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>616323</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="829235" y="2588559"/>
+          <a:ext cx="3989294" cy="1512794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>Apptitude : profit and loss</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>  Time: 5 p.m to 6 p.m</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1180,7 +1255,7 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1368,9 @@
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -1334,7 +1411,9 @@
       <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1364,10 +1443,11 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:AE2 C2:C3 F3:AE3 D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:AE3">
       <formula1>"Present, Absent,Reason"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
6  february Presenti sheet
6  february Presenti sheet
</commit_message>
<xml_diff>
--- a/Java B10 G1.xlsx
+++ b/Java B10 G1.xlsx
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="9">
   <si>
     <t>Student Name</t>
   </si>
@@ -442,15 +442,12 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
-            <a:t>Apptitude : profit and loss</a:t>
-          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
-            <a:t>  Time: 5 p.m to 6 p.m</a:t>
+            <a:t>  Time: 5 p.m to 7 p.m</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1255,7 +1252,7 @@
   <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1371,9 +1368,15 @@
       <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -1414,9 +1417,15 @@
       <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>

</xml_diff>